<commit_message>
testing b2b v1 revisi
</commit_message>
<xml_diff>
--- a/downloads/Template-Cart.xlsx
+++ b/downloads/Template-Cart.xlsx
@@ -2,8 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R8e295ecf434349b0"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="2" r:id="R6f7cff0a74fc40fe"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R9e023b43d0c94872"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="2" r:id="Rbdedee5a48d64be8"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -192,7 +192,7 @@
         <x:v>12-100020-00000</x:v>
       </x:c>
       <x:c r="C4" s="6" t="n">
-        <x:v>600</x:v>
+        <x:v>660</x:v>
       </x:c>
       <x:c r="D4" s="4" t="str">
         <x:v>Contoh SKU</x:v>
@@ -206,7 +206,7 @@
         <x:v>12-100020-FLAP</x:v>
       </x:c>
       <x:c r="C5" s="6" t="n">
-        <x:v>1000</x:v>
+        <x:v>1100</x:v>
       </x:c>
       <x:c r="D5" s="4" t="str">
         <x:v>Contoh SKU</x:v>
@@ -220,7 +220,7 @@
         <x:v>12-50012-00000</x:v>
       </x:c>
       <x:c r="C6" s="6" t="n">
-        <x:v>1600</x:v>
+        <x:v>1700</x:v>
       </x:c>
       <x:c r="D6" s="4" t="str">
         <x:v>Contoh SKU</x:v>

</xml_diff>

<commit_message>
modif code and run with node main.js
</commit_message>
<xml_diff>
--- a/downloads/Template-Cart.xlsx
+++ b/downloads/Template-Cart.xlsx
@@ -2,8 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rd20c2d7301624f73"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="2" r:id="Rfb7f46860817476f"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rd37273c9c036402b"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="2" r:id="R78177af1d85d4fb0"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -161,10 +161,10 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="B2" s="4" t="str">
-        <x:v>11-12H410090P43TC</x:v>
+        <x:v>11-GTZ-7VMF</x:v>
       </x:c>
       <x:c r="C2" s="6" t="n">
-        <x:v>2</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D2" s="4" t="str">
         <x:v>Contoh SKU</x:v>
@@ -175,10 +175,10 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B3" s="4" t="str">
-        <x:v>11-GTZ-7VMF</x:v>
+        <x:v>11-H12V3530H5</x:v>
       </x:c>
       <x:c r="C3" s="6" t="n">
-        <x:v>10</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D3" s="4" t="str">
         <x:v>Contoh SKU</x:v>
@@ -189,10 +189,10 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B4" s="4" t="str">
-        <x:v>11-H12V3530H5</x:v>
+        <x:v>12-100020-00000</x:v>
       </x:c>
       <x:c r="C4" s="6" t="n">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D4" s="4" t="str">
         <x:v>Contoh SKU</x:v>
@@ -203,10 +203,10 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B5" s="4" t="str">
-        <x:v>12-100020-00000</x:v>
+        <x:v>12-100020-FLAP</x:v>
       </x:c>
       <x:c r="C5" s="6" t="n">
-        <x:v>1115</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="D5" s="4" t="str">
         <x:v>Contoh SKU</x:v>
@@ -217,10 +217,10 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="B6" s="4" t="str">
-        <x:v>12-100020-FLAP</x:v>
+        <x:v>12-50012-00000</x:v>
       </x:c>
       <x:c r="C6" s="6" t="n">
-        <x:v>1900</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="D6" s="4" t="str">
         <x:v>Contoh SKU</x:v>
@@ -231,10 +231,10 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B7" s="4" t="str">
-        <x:v>12-27517-AT601X</x:v>
+        <x:v>FP-06435-KPP-2700</x:v>
       </x:c>
       <x:c r="C7" s="6" t="n">
-        <x:v>10</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="D7" s="4" t="str">
         <x:v>Contoh SKU</x:v>
@@ -245,10 +245,10 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B8" s="4" t="str">
-        <x:v>12-50012-00000</x:v>
+        <x:v>FP-43120-362-2700</x:v>
       </x:c>
       <x:c r="C8" s="6" t="n">
-        <x:v>2506</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="D8" s="4" t="str">
         <x:v>Contoh SKU</x:v>
@@ -259,10 +259,10 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="B9" s="4" t="str">
-        <x:v>FP-06435-KPP-2700</x:v>
+        <x:v>FP-43125-KGA-2700</x:v>
       </x:c>
       <x:c r="C9" s="6" t="n">
-        <x:v>31</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="D9" s="4" t="str">
         <x:v>Contoh SKU</x:v>
@@ -273,10 +273,10 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="B10" s="4" t="str">
-        <x:v>FP-F54P8-JMX-222C</x:v>
+        <x:v>FP-54410-THU-2700</x:v>
       </x:c>
       <x:c r="C10" s="6" t="n">
-        <x:v>10</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="D10" s="4" t="str">
         <x:v>Contoh SKU</x:v>
@@ -287,10 +287,10 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="B11" s="4" t="str">
-        <x:v>FP-H1801-MIO-2100</x:v>
+        <x:v>FP-F533A-RXK-2700</x:v>
       </x:c>
       <x:c r="C11" s="6" t="n">
-        <x:v>10</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="D11" s="4" t="str">
         <x:v>Contoh SKU</x:v>
@@ -301,10 +301,10 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="B12" s="4" t="str">
-        <x:v>GSMF-GTZ-4V</x:v>
+        <x:v>FP-W0045-F1Z-2700</x:v>
       </x:c>
       <x:c r="C12" s="6" t="n">
-        <x:v>26</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="D12" s="4" t="str">
         <x:v>Contoh SKU</x:v>
@@ -315,10 +315,10 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="B13" s="4" t="str">
-        <x:v>GSMF-GTZ-5S</x:v>
+        <x:v>GSMF-GTZ-4V</x:v>
       </x:c>
       <x:c r="C13" s="6" t="n">
-        <x:v>1</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="D13" s="4" t="str">
         <x:v>Contoh SKU</x:v>
@@ -329,26 +329,12 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="B14" s="4" t="str">
-        <x:v>TO-15601-AVZ-1800</x:v>
+        <x:v>H2-231PA-KZL-1200</x:v>
       </x:c>
       <x:c r="C14" s="6" t="n">
-        <x:v>8</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="D14" s="4" t="str">
-        <x:v>Contoh SKU</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15">
-      <x:c r="A15" s="6" t="n">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="B15" s="4" t="str">
-        <x:v>TO-48510-GRE-1700</x:v>
-      </x:c>
-      <x:c r="C15" s="6" t="n">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="D15" s="4" t="str">
         <x:v>Contoh SKU</x:v>
       </x:c>
     </x:row>

</xml_diff>